<commit_message>
opmize game page, added tips and gallery language
</commit_message>
<xml_diff>
--- a/cfg/excel/article_cfg.xlsx
+++ b/cfg/excel/article_cfg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Emanon\cfg\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0B1DBB-1F77-4ADF-A6E7-E7A2098FE00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCBB3E3-FAA4-4E72-821C-B0FD054CD33E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -545,11 +545,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21:C21"/>
+      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -724,52 +724,7 @@
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="2">
-        <v>8</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" s="2">
-        <v>9</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="2">
-        <v>10</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" s="2" t="s">
+      <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>